<commit_message>
Adding assert country testcases and integrate ExtentReport
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farha\IdeaProjects\Ecommerce\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F6713D0-D59D-4129-A116-833B8C8DD480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFFE534-221B-4753-ADA0-77B543212D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12" yWindow="12" windowWidth="23016" windowHeight="12216" activeTab="1" xr2:uid="{3C8CE09A-A673-49DA-87D0-31801A7C4ADE}"/>
+    <workbookView xWindow="12" yWindow="12" windowWidth="23016" windowHeight="12216" xr2:uid="{3C8CE09A-A673-49DA-87D0-31801A7C4ADE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Username</t>
   </si>
@@ -45,12 +45,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>testlumaqa@mailinator.com</t>
-  </si>
-  <si>
-    <t>Luma12345</t>
-  </si>
-  <si>
     <t>Luma12345a</t>
   </si>
   <si>
@@ -91,13 +85,82 @@
   </si>
   <si>
     <t>Hoodie</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>ZipCode</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phone </t>
+  </si>
+  <si>
+    <t>FakeCompany</t>
+  </si>
+  <si>
+    <t>AbcTest</t>
+  </si>
+  <si>
+    <t>Abc Block 4</t>
+  </si>
+  <si>
+    <t>Test Street 3</t>
+  </si>
+  <si>
+    <t>Calgary</t>
+  </si>
+  <si>
+    <t>Manchester</t>
+  </si>
+  <si>
+    <t>AB12 3CD</t>
+  </si>
+  <si>
+    <t>XY42 0BC</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>England</t>
+  </si>
+  <si>
+    <t>Fname</t>
+  </si>
+  <si>
+    <t>Lname</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Dummy</t>
+  </si>
+  <si>
+    <t>lumaQA@mailinator.com</t>
+  </si>
+  <si>
+    <t>Test@12345</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +175,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -135,9 +204,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -473,46 +543,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{654769DD-6CE7-49CF-9F6C-94305E0DC5B9}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.44140625" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2">
+        <v>123456789</v>
+      </c>
+      <c r="I2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3">
+        <v>987654321</v>
+      </c>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{0F15F1AA-AD9A-4A01-BCF9-3A67B5B60B7F}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{F4D8D402-E1FA-43DB-B514-A143E1D92763}"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{F4D8D402-E1FA-43DB-B514-A143E1D92763}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{3D1359FB-EFBC-43C0-9482-40BB82279929}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -522,7 +668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ACBD3AE-87F4-4E06-BD6B-018D0B86D44A}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -535,50 +681,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>